<commit_message>
tests for groups update
</commit_message>
<xml_diff>
--- a/khppp/testData.xlsx
+++ b/khppp/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -54,15 +54,6 @@
     <t>LabManager111</t>
   </si>
   <si>
-    <t>Incorrect login or password</t>
-  </si>
-  <si>
-    <t>Admin Admin (ADMIN)</t>
-  </si>
-  <si>
-    <t>LabManager LabManager (LAB_MANAGER)</t>
-  </si>
-  <si>
     <t>users</t>
   </si>
   <si>
@@ -108,7 +99,13 @@
     <t>sashaa</t>
   </si>
   <si>
-    <t>OstrTestGroup4</t>
+    <t>Admin Admin (admin)</t>
+  </si>
+  <si>
+    <t>LabManager LabManager (lab manager)</t>
+  </si>
+  <si>
+    <t>OstrTestGroup5</t>
   </si>
 </sst>
 </file>
@@ -453,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +487,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -504,7 +501,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -517,16 +514,13 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -567,7 +561,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -581,7 +575,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -590,10 +584,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -606,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,15 +625,15 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -650,7 +644,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -661,7 +655,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -670,15 +664,15 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -687,12 +681,12 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -701,10 +695,10 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test for Groups 3
</commit_message>
<xml_diff>
--- a/khppp/testData.xlsx
+++ b/khppp/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>OstrTestGroup5</t>
+  </si>
+  <si>
+    <t>Incorrect login or password</t>
   </si>
 </sst>
 </file>
@@ -514,6 +517,9 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
test for Groups 4
</commit_message>
<xml_diff>
--- a/khppp/testData.xlsx
+++ b/khppp/testData.xlsx
@@ -108,7 +108,7 @@
     <t>Sorry, something terrible happened to server.</t>
   </si>
   <si>
-    <t>OstrTestGroup6</t>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>